<commit_message>
Did some research on node-link diagrams and added in document + in time sheet
</commit_message>
<xml_diff>
--- a/docs/Group29_timesheets.xlsx
+++ b/docs/Group29_timesheets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20172072\Documents\GitHub\Ceres29\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF61EEC3-DF6E-46BE-AE27-DEB7EF2C2F64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD2CFAA-7D0E-4532-9288-E3EE52529853}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{3DDC6BD7-6872-42DD-BCD4-E5569E459740}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
   <si>
     <t>Time sheets</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>When</t>
+  </si>
+  <si>
+    <t>Search different options for tree-node diagram</t>
   </si>
 </sst>
 </file>
@@ -279,12 +282,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -296,6 +293,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -312,12 +321,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -637,90 +640,88 @@
   <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="59.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.109375" customWidth="1"/>
-    <col min="5" max="9" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="24"/>
     </row>
     <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="21"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="5"/>
-      <c r="L3" s="23" t="s">
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="16"/>
+      <c r="L3" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="24"/>
+      <c r="M3" s="18"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="4" t="s">
         <v>26</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="9" t="s">
         <v>3</v>
       </c>
       <c r="M4" s="3">
@@ -729,34 +730,34 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="6">
         <v>43579</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="8">
         <v>2</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="8">
         <v>2</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="8">
         <v>2</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="8">
         <v>2</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="8">
         <v>2</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="8">
         <v>2</v>
       </c>
       <c r="I5" s="2">
         <v>2</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="L5" s="9" t="s">
         <v>17</v>
       </c>
       <c r="M5" s="3">
@@ -765,34 +766,34 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="6">
         <v>43579</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="8">
         <v>0.5</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="8">
         <v>0.5</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="8">
         <v>0.5</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="8">
         <v>0.5</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="8">
         <v>0.5</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="8">
         <v>0.5</v>
       </c>
       <c r="I6" s="2">
         <v>0.5</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="9" t="s">
         <v>2</v>
       </c>
       <c r="M6" s="3">
@@ -801,22 +802,22 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="6">
         <v>43579</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7">
-        <v>1</v>
-      </c>
-      <c r="H7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="H7" s="5"/>
       <c r="I7" s="3"/>
-      <c r="L7" s="11" t="s">
+      <c r="L7" s="9" t="s">
         <v>19</v>
       </c>
       <c r="M7" s="3">
@@ -825,46 +826,46 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="7">
         <v>43579</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="5">
         <v>0.1</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
       <c r="I8" s="3"/>
-      <c r="L8" s="11" t="s">
+      <c r="L8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="M8" s="3">
         <f>140-SUM(G1:G10006)</f>
-        <v>136.5</v>
+        <v>134.75</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="7">
         <v>43579</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5">
         <v>0.2</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
       <c r="I9" s="3"/>
-      <c r="L9" s="11" t="s">
+      <c r="L9" s="9" t="s">
         <v>14</v>
       </c>
       <c r="M9" s="3">
@@ -873,182 +874,188 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="7">
         <v>43579</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="5">
         <v>1</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="5">
         <v>1</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
       <c r="I10" s="3"/>
-      <c r="L10" s="12" t="s">
+      <c r="L10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="M10" s="13">
+      <c r="M10" s="11">
         <f>140-SUM(I1:I10006)</f>
         <v>137.5</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="7">
         <v>43579</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7">
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5">
         <v>1</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="5">
         <v>1</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="7">
         <v>43579</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7">
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5">
         <v>1</v>
       </c>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="A13" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="7">
+        <v>43580</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5">
+        <v>1.25</v>
+      </c>
+      <c r="H13" s="5"/>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="16"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="3"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
       <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="16"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="16"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="16"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="19"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="21"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="5"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="16"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="16"/>
+      <c r="A21" s="14"/>
       <c r="B21" s="3"/>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="4" t="s">
         <v>26</v>
       </c>
       <c r="I21" s="1" t="s">
@@ -1056,87 +1063,87 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="16"/>
+      <c r="A22" s="14"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="16"/>
+      <c r="A23" s="14"/>
       <c r="B23" s="3"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="16"/>
+      <c r="A24" s="14"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="19"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="21"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="5"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="16"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="16"/>
+      <c r="A27" s="14"/>
       <c r="B27" s="3"/>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G27" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="H27" s="4" t="s">
         <v>26</v>
       </c>
       <c r="I27" s="1" t="s">
@@ -1144,87 +1151,87 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="16"/>
+      <c r="A28" s="14"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="16"/>
+      <c r="A29" s="14"/>
       <c r="B29" s="3"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="16"/>
+      <c r="A30" s="14"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
       <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="19"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="21"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="5"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="16"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="16"/>
+      <c r="A33" s="14"/>
       <c r="B33" s="3"/>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E33" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F33" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G33" s="6" t="s">
+      <c r="G33" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H33" s="6" t="s">
+      <c r="H33" s="4" t="s">
         <v>26</v>
       </c>
       <c r="I33" s="1" t="s">
@@ -1232,84 +1239,86 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="16"/>
+      <c r="A34" s="14"/>
       <c r="B34" s="3"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
       <c r="I34" s="3"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="16"/>
+      <c r="A35" s="14"/>
       <c r="B35" s="3"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
       <c r="I35" s="3"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="16"/>
+      <c r="A36" s="14"/>
       <c r="B36" s="3"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
       <c r="I36" s="3"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="16"/>
+      <c r="A37" s="14"/>
       <c r="B37" s="3"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
       <c r="I37" s="3"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="16"/>
+      <c r="A38" s="14"/>
       <c r="B38" s="3"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
       <c r="I38" s="3"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="16"/>
+      <c r="A39" s="14"/>
       <c r="B39" s="3"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
       <c r="I39" s="3"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A1:I1"/>
     <mergeCell ref="C32:I32"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="A19:I19"/>
@@ -1318,8 +1327,6 @@
     <mergeCell ref="C20:I20"/>
     <mergeCell ref="C26:I26"/>
     <mergeCell ref="C3:I3"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added references and updated timesheet
</commit_message>
<xml_diff>
--- a/docs/Group29_timesheets.xlsx
+++ b/docs/Group29_timesheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21617"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel\Documents\Ceres29\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20181813\Documents\Studie\2018-2019\2IOA0 - DBL\Repo\Ceres29\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1654B21-1867-4149-B599-83D9BB665946}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B4F9A7-1DA7-4A81-9ED9-A599D074095B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5640" xr2:uid="{3DDC6BD7-6872-42DD-BCD4-E5569E459740}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" xr2:uid="{3DDC6BD7-6872-42DD-BCD4-E5569E459740}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,14 +23,35 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={8D192B17-B68B-403F-9072-B7EA43C4C837}</author>
+  </authors>
+  <commentList>
+    <comment ref="A16" authorId="0" shapeId="0" xr:uid="{8D192B17-B68B-403F-9072-B7EA43C4C837}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    I suppose at least a few did this, so I think it's easiest if you just add your hours to this row</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
   <si>
     <t>Time sheets</t>
   </si>
@@ -132,13 +153,16 @@
   </si>
   <si>
     <t>Rounding up p5 implementation to function as an example</t>
+  </si>
+  <si>
+    <t>Looking up and reading references project description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +185,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -331,7 +361,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -346,8 +376,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Rink Pieters" id="{D24A8A3B-3988-40E5-BB15-ADA6B2156A11}" userId="Rink Pieters" providerId="None"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -641,22 +677,30 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A16" dT="2019-04-25T15:05:17.04" personId="{D24A8A3B-3988-40E5-BB15-ADA6B2156A11}" id="{8D192B17-B68B-403F-9072-B7EA43C4C837}">
+    <text>I suppose at least a few did this, so I think it's easiest if you just add your hours to this row</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB5D6305-FF9A-482B-B9AA-9E4647F19C0A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB5D6305-FF9A-482B-B9AA-9E4647F19C0A}">
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="59.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="9" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="18.350000000000001" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -669,7 +713,7 @@
       <c r="H1" s="19"/>
       <c r="I1" s="20"/>
     </row>
-    <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="18.350000000000001" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
         <v>6</v>
       </c>
@@ -682,7 +726,7 @@
       <c r="H2" s="16"/>
       <c r="I2" s="17"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
@@ -703,7 +747,7 @@
       </c>
       <c r="M3" s="24"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -735,7 +779,7 @@
         <v>136.4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>28</v>
       </c>
@@ -771,7 +815,7 @@
         <v>136.5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>29</v>
       </c>
@@ -807,7 +851,7 @@
         <v>136.30000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>11</v>
       </c>
@@ -831,7 +875,7 @@
         <v>131.5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>4</v>
       </c>
@@ -855,7 +899,7 @@
         <v>134.75</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>5</v>
       </c>
@@ -876,10 +920,10 @@
       </c>
       <c r="M9" s="3">
         <f>140-SUM(H1:H10007)</f>
-        <v>136.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>13</v>
       </c>
@@ -905,7 +949,7 @@
         <v>137.5</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>12</v>
       </c>
@@ -924,7 +968,7 @@
       <c r="H11" s="5"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>32</v>
       </c>
@@ -941,7 +985,7 @@
       <c r="H12" s="5"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
         <v>15</v>
       </c>
@@ -958,7 +1002,7 @@
       </c>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>31</v>
       </c>
@@ -975,7 +1019,7 @@
       <c r="H14" s="5"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>33</v>
       </c>
@@ -992,18 +1036,24 @@
       <c r="H15" s="5"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="3"/>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="7">
+        <v>43580</v>
+      </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
+      <c r="H16" s="5">
+        <v>1.5</v>
+      </c>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="3"/>
       <c r="C17" s="5"/>
@@ -1014,7 +1064,7 @@
       <c r="H17" s="5"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="3"/>
       <c r="C18" s="5"/>
@@ -1025,7 +1075,7 @@
       <c r="H18" s="5"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="3"/>
       <c r="C19" s="5"/>
@@ -1036,7 +1086,7 @@
       <c r="H19" s="5"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="18.350000000000001" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
         <v>7</v>
       </c>
@@ -1049,7 +1099,7 @@
       <c r="H20" s="16"/>
       <c r="I20" s="17"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>1</v>
       </c>
@@ -1066,7 +1116,7 @@
       <c r="H21" s="21"/>
       <c r="I21" s="22"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4" t="s">
@@ -1091,7 +1141,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
@@ -1102,7 +1152,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
@@ -1113,7 +1163,7 @@
       <c r="H24" s="4"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="B25" s="3"/>
       <c r="C25" s="5"/>
@@ -1124,7 +1174,7 @@
       <c r="H25" s="5"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="18.350000000000001" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
         <v>8</v>
       </c>
@@ -1137,7 +1187,7 @@
       <c r="H26" s="16"/>
       <c r="I26" s="17"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
         <v>1</v>
       </c>
@@ -1154,7 +1204,7 @@
       <c r="H27" s="21"/>
       <c r="I27" s="22"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="B28" s="3"/>
       <c r="C28" s="4" t="s">
@@ -1179,7 +1229,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="3"/>
       <c r="C29" s="4"/>
@@ -1190,7 +1240,7 @@
       <c r="H29" s="4"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="14"/>
       <c r="B30" s="3"/>
       <c r="C30" s="4"/>
@@ -1201,7 +1251,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="14"/>
       <c r="B31" s="3"/>
       <c r="C31" s="5"/>
@@ -1212,7 +1262,7 @@
       <c r="H31" s="5"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="18.350000000000001" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
         <v>9</v>
       </c>
@@ -1225,7 +1275,7 @@
       <c r="H32" s="16"/>
       <c r="I32" s="17"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
         <v>1</v>
       </c>
@@ -1242,7 +1292,7 @@
       <c r="H33" s="21"/>
       <c r="I33" s="22"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="14"/>
       <c r="B34" s="3"/>
       <c r="C34" s="4" t="s">
@@ -1267,7 +1317,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="14"/>
       <c r="B35" s="3"/>
       <c r="C35" s="5"/>
@@ -1278,7 +1328,7 @@
       <c r="H35" s="5"/>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="14"/>
       <c r="B36" s="3"/>
       <c r="C36" s="5"/>
@@ -1289,7 +1339,7 @@
       <c r="H36" s="5"/>
       <c r="I36" s="3"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="14"/>
       <c r="B37" s="3"/>
       <c r="C37" s="5"/>
@@ -1300,7 +1350,7 @@
       <c r="H37" s="5"/>
       <c r="I37" s="3"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="14"/>
       <c r="B38" s="3"/>
       <c r="C38" s="5"/>
@@ -1311,7 +1361,7 @@
       <c r="H38" s="5"/>
       <c r="I38" s="3"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="14"/>
       <c r="B39" s="3"/>
       <c r="C39" s="5"/>
@@ -1322,7 +1372,7 @@
       <c r="H39" s="5"/>
       <c r="I39" s="3"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="14"/>
       <c r="B40" s="3"/>
       <c r="C40" s="5"/>
@@ -1333,7 +1383,7 @@
       <c r="H40" s="5"/>
       <c r="I40" s="3"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -1359,5 +1409,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>